<commit_message>
sql script is added in database folder
</commit_message>
<xml_diff>
--- a/Documentation/ERD_Project_Tanders_20140904.xlsx
+++ b/Documentation/ERD_Project_Tanders_20140904.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iggy\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13620" windowHeight="15560"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
     <sheet name="Diagram" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -1273,7 +1271,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1331,7 +1329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1366,7 +1364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1543,7 +1541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1553,19 +1551,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1573,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1585,7 +1583,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1599,7 +1597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1613,7 +1611,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1627,7 +1625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1641,7 +1639,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1655,7 +1653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
@@ -1669,7 +1667,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1683,7 +1681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1697,7 +1695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1711,7 +1709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1719,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1729,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1745,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1759,7 +1757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1773,7 +1771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1785,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -1801,7 +1799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1815,7 +1813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1829,7 +1827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1843,10 +1841,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1856,7 +1854,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1866,7 +1864,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +1878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="28">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="28">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1908,7 +1906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="28">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1922,7 +1920,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="28">
       <c r="A31" s="2" t="s">
         <v>50</v>
       </c>
@@ -1936,7 +1934,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="28">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1950,7 +1948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1964,7 +1962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1978,7 +1976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1992,10 +1990,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +2003,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -2015,7 +2013,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -2043,7 +2041,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2057,7 +2055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2071,7 +2069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2085,7 +2083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -2099,7 +2097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>27</v>
       </c>
@@ -2113,7 +2111,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -2123,7 +2121,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -2133,7 +2131,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
@@ -2147,7 +2145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="28">
       <c r="A50" s="2" t="s">
         <v>18</v>
       </c>
@@ -2161,7 +2159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>35</v>
       </c>
@@ -2175,7 +2173,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="28">
       <c r="A52" s="2" t="s">
         <v>48</v>
       </c>
@@ -2189,7 +2187,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
@@ -2203,7 +2201,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -2217,7 +2215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -2231,7 +2229,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>27</v>
       </c>
@@ -2245,7 +2243,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +2253,7 @@
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>1</v>
       </c>
@@ -2265,7 +2263,7 @@
       <c r="C59" s="3"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>2</v>
       </c>
@@ -2279,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="28">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -2293,7 +2291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="28">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -2307,7 +2305,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="28">
       <c r="A63" t="s">
         <v>40</v>
       </c>
@@ -2321,7 +2319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="28">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="28">
       <c r="A65" t="s">
         <v>50</v>
       </c>
@@ -2349,7 +2347,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>22</v>
       </c>
@@ -2363,7 +2361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -2377,7 +2375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>27</v>
       </c>
@@ -2393,7 +2391,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2405,9 +2407,14 @@
       <selection activeCell="AM6" sqref="AM6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>